<commit_message>
Update c=indices sociaux: style
</commit_message>
<xml_diff>
--- a/shared_data/moyen_indices.xlsx
+++ b/shared_data/moyen_indices.xlsx
@@ -475,7 +475,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -523,10 +523,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>35</v>
+        <v>4.8</v>
       </c>
       <c r="C4" s="4">
-        <v>20</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1">

</xml_diff>

<commit_message>
Update: add moy_pro, adjust color
</commit_message>
<xml_diff>
--- a/shared_data/moyen_indices.xlsx
+++ b/shared_data/moyen_indices.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>002</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>code</t>
+  </si>
+  <si>
+    <t>moy_pro</t>
   </si>
 </sst>
 </file>
@@ -472,20 +475,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="5"/>
-    <col min="2" max="2" width="45.44140625" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1">
+    <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -495,30 +496,39 @@
       <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1">
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>35</v>
+        <v>41.6</v>
       </c>
       <c r="C2" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1">
+        <v>37.6</v>
+      </c>
+      <c r="D2" s="4">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>45</v>
+        <v>21.3</v>
       </c>
       <c r="C3" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1">
+        <v>30.4</v>
+      </c>
+      <c r="D3" s="4">
+        <v>35.700000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -528,137 +538,170 @@
       <c r="C4" s="4">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1">
+      <c r="D4" s="4">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>45</v>
+        <v>6.8</v>
       </c>
       <c r="C5" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1">
+        <v>8.4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D6" s="4">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C7" s="4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4">
-        <v>11</v>
+        <v>4.8</v>
       </c>
       <c r="C8" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1">
+        <v>5.2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="4">
-        <v>45</v>
+        <v>14.6</v>
       </c>
       <c r="C9" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1">
+        <v>17.2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="4">
-        <v>5</v>
+        <v>2.8</v>
       </c>
       <c r="C10" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1">
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="4">
-        <v>30</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C11" s="4">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D11" s="4">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4">
-        <v>45</v>
+        <v>12.1</v>
       </c>
       <c r="C12" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1">
+        <v>11.9</v>
+      </c>
+      <c r="D12" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
-        <v>45</v>
-      </c>
-      <c r="C13" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="4">
-        <v>20</v>
+        <v>10.7</v>
       </c>
       <c r="C15" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" thickBot="1">
+        <v>7.1</v>
+      </c>
+      <c r="D15" s="4">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="4">
-        <v>45</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C16" s="4">
-        <v>25</v>
+        <v>4.5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: test nv approche
</commit_message>
<xml_diff>
--- a/shared_data/moyen_indices.xlsx
+++ b/shared_data/moyen_indices.xlsx
@@ -16,52 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>005</t>
-  </si>
-  <si>
-    <t>006</t>
-  </si>
-  <si>
-    <t>007</t>
-  </si>
-  <si>
-    <t>008</t>
-  </si>
-  <si>
-    <t>009</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>011</t>
-  </si>
-  <si>
-    <t>012</t>
-  </si>
-  <si>
-    <t>013</t>
-  </si>
-  <si>
-    <t>014</t>
-  </si>
-  <si>
-    <t>015</t>
-  </si>
-  <si>
-    <t>016</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>moy_nat</t>
   </si>
@@ -73,6 +28,81 @@
   </si>
   <si>
     <t>moy_pro</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
 </sst>
 </file>
@@ -139,9 +169,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -152,12 +180,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -174,13 +206,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,237 +507,426 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3">
+        <v>41.6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>37.6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>21.3</v>
+      </c>
+      <c r="C3" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="D3" s="3">
+        <v>35.700000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="D4" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8.4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C6" s="3">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D6" s="3">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>17.2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1">
+      <c r="A11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C11" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D11" s="3">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1">
+      <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B13" s="3">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <v>20</v>
+      </c>
+      <c r="D13" s="3">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1">
+      <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B14" s="3">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3">
+        <v>20</v>
+      </c>
+      <c r="D14" s="3">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1">
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3">
+        <v>10.7</v>
+      </c>
+      <c r="C15" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1">
+      <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="B16" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1">
+      <c r="A17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="3">
         <v>41.6</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C17" s="3">
         <v>37.6</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D17" s="3">
         <v>32.4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
+    <row r="18" spans="1:4" ht="15" thickBot="1">
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3">
         <v>21.3</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C18" s="3">
         <v>30.4</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D18" s="3">
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1">
-      <c r="A4" s="3" t="s">
+    <row r="19" spans="1:4" ht="15" thickBot="1">
+      <c r="A19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="C19" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="D19" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1">
+      <c r="A20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="C20" s="3">
+        <v>8.4</v>
+      </c>
+      <c r="D20" s="3">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1">
+      <c r="A21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="3">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D21" s="3">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1">
+      <c r="A22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1">
+      <c r="A23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="C23" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1">
+      <c r="A24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="C24" s="3">
+        <v>17.2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1">
+      <c r="A25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
-        <v>4.8</v>
-      </c>
-      <c r="C4" s="4">
-        <v>5.9</v>
-      </c>
-      <c r="D4" s="4">
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1">
+      <c r="A26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>6.8</v>
-      </c>
-      <c r="C5" s="4">
-        <v>8.4</v>
-      </c>
-      <c r="D5" s="4">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
-        <v>17</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="C26" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D26" s="3">
         <v>20.399999999999999</v>
       </c>
-      <c r="D6" s="4">
-        <v>26.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4">
-        <v>4.8</v>
-      </c>
-      <c r="C8" s="4">
-        <v>5.2</v>
-      </c>
-      <c r="D8" s="4">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4">
-        <v>14.6</v>
-      </c>
-      <c r="C9" s="4">
-        <v>17.2</v>
-      </c>
-      <c r="D9" s="4">
-        <v>27.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="C10" s="4">
-        <v>3</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1">
-      <c r="A11" s="3" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="15" thickBot="1">
+      <c r="A27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="D27" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="C11" s="4">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="D11" s="4">
-        <v>20.399999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1">
-      <c r="A12" s="3" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="15" thickBot="1">
+      <c r="A28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
-        <v>12.1</v>
-      </c>
-      <c r="C12" s="4">
-        <v>11.9</v>
-      </c>
-      <c r="D12" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4">
+      <c r="C28" s="3">
+        <v>20</v>
+      </c>
+      <c r="D28" s="3">
         <v>20.2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4">
+    <row r="29" spans="1:4" ht="15" thickBot="1">
+      <c r="A29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3">
         <v>10</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C29" s="3">
         <v>20</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4">
-        <v>10.7</v>
-      </c>
-      <c r="C15" s="4">
-        <v>7.1</v>
-      </c>
-      <c r="D15" s="4">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C16" s="4">
-        <v>4.5</v>
-      </c>
-      <c r="D16" s="4">
-        <v>3</v>
+      <c r="D29" s="3">
+        <v>20.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update: test nv données
</commit_message>
<xml_diff>
--- a/shared_data/moyen_indices.xlsx
+++ b/shared_data/moyen_indices.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>moy_nat</t>
   </si>
@@ -55,54 +55,6 @@
   </si>
   <si>
     <t>09</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
   </si>
 </sst>
 </file>
@@ -180,16 +132,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -510,7 +460,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -537,13 +487,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>41.6</v>
+        <v>6.8</v>
       </c>
       <c r="C2" s="3">
-        <v>37.6</v>
+        <v>8.4</v>
       </c>
       <c r="D2" s="3">
-        <v>32.4</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1">
@@ -551,13 +501,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>21.3</v>
+        <v>11.9</v>
       </c>
       <c r="C3" s="3">
-        <v>30.4</v>
+        <v>13.5</v>
       </c>
       <c r="D3" s="3">
-        <v>35.700000000000003</v>
+        <v>19.7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1">
@@ -568,10 +518,10 @@
         <v>4.8</v>
       </c>
       <c r="C4" s="3">
-        <v>5.9</v>
+        <v>5.2</v>
       </c>
       <c r="D4" s="3">
-        <v>8.3000000000000007</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1">
@@ -579,13 +529,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="3">
-        <v>6.8</v>
+        <v>14.6</v>
       </c>
       <c r="C5" s="3">
-        <v>8.4</v>
+        <v>17.2</v>
       </c>
       <c r="D5" s="3">
-        <v>11.2</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1">
@@ -621,13 +571,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="3">
-        <v>4.8</v>
+        <v>2.8</v>
       </c>
       <c r="C8" s="3">
-        <v>5.2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="3">
-        <v>4.5999999999999996</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1">
@@ -635,13 +585,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="3">
-        <v>14.6</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C9" s="3">
-        <v>17.2</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D9" s="3">
-        <v>27.2</v>
+        <v>20.399999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1">
@@ -649,279 +599,279 @@
         <v>12</v>
       </c>
       <c r="B10" s="3">
-        <v>2.8</v>
+        <v>12.1</v>
       </c>
       <c r="C10" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="D10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>10.7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="D12" s="3">
         <v>3</v>
       </c>
-      <c r="D10" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1">
-      <c r="A11" s="5" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>56.5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>51.9</v>
+      </c>
+      <c r="D13" s="3">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B14" s="3">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3">
+        <v>21.2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>26.6</v>
+      </c>
+      <c r="C15" s="3">
+        <v>25.1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>53.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="D16" s="3">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="C17" s="3">
+        <v>65.7</v>
+      </c>
+      <c r="D17" s="3">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3">
+        <v>16.2</v>
+      </c>
+      <c r="D18" s="3">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="C19" s="3">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D19" s="3">
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>62.8</v>
+      </c>
+      <c r="C21" s="3">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="D21" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="C22" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="D22" s="3">
         <v>8.3000000000000007</v>
       </c>
-      <c r="C11" s="3">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="D11" s="3">
-        <v>20.399999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1">
-      <c r="A12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3">
-        <v>12.1</v>
-      </c>
-      <c r="C12" s="3">
-        <v>11.9</v>
-      </c>
-      <c r="D12" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1">
-      <c r="A13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="3">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3">
-        <v>20.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1">
-      <c r="A14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3">
-        <v>20</v>
-      </c>
-      <c r="D14" s="3">
-        <v>20.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1">
-      <c r="A15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3">
-        <v>10.7</v>
-      </c>
-      <c r="C15" s="3">
-        <v>7.1</v>
-      </c>
-      <c r="D15" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1">
-      <c r="A16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C16" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="D16" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1">
-      <c r="A17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="3">
-        <v>41.6</v>
-      </c>
-      <c r="C17" s="3">
-        <v>37.6</v>
-      </c>
-      <c r="D17" s="3">
-        <v>32.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1">
-      <c r="A18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="3">
-        <v>21.3</v>
-      </c>
-      <c r="C18" s="3">
-        <v>30.4</v>
-      </c>
-      <c r="D18" s="3">
-        <v>35.700000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1">
-      <c r="A19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="3">
-        <v>4.8</v>
-      </c>
-      <c r="C19" s="3">
-        <v>5.9</v>
-      </c>
-      <c r="D19" s="3">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1">
-      <c r="A20" s="5" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B20" s="3">
-        <v>6.8</v>
-      </c>
-      <c r="C20" s="3">
-        <v>8.4</v>
-      </c>
-      <c r="D20" s="3">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1">
-      <c r="A21" s="5" t="s">
+      <c r="B23" s="3">
+        <v>24.8</v>
+      </c>
+      <c r="C23" s="3">
+        <v>28.3</v>
+      </c>
+      <c r="D23" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B21" s="3">
-        <v>17</v>
-      </c>
-      <c r="C21" s="3">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="D21" s="3">
-        <v>26.7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1">
-      <c r="A22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1">
-      <c r="A23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3">
-        <v>4.8</v>
-      </c>
-      <c r="C23" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="D23" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1">
-      <c r="A24" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="B24" s="3">
-        <v>14.6</v>
+        <v>95.8</v>
       </c>
       <c r="C24" s="3">
-        <v>17.2</v>
+        <v>95</v>
       </c>
       <c r="D24" s="3">
-        <v>27.2</v>
+        <v>95.9</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" thickBot="1">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="B25" s="3">
-        <v>2.8</v>
+        <v>1.7</v>
       </c>
       <c r="C25" s="3">
-        <v>3</v>
+        <v>1.7</v>
       </c>
       <c r="D25" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" thickBot="1">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>8.3000000000000007</v>
+        <v>26.8</v>
       </c>
       <c r="C26" s="3">
-        <v>8.6999999999999993</v>
+        <v>28.8</v>
       </c>
       <c r="D26" s="3">
-        <v>20.399999999999999</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" thickBot="1">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="3">
-        <v>12.1</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="C27" s="3">
-        <v>11.9</v>
+        <v>16.8</v>
       </c>
       <c r="D27" s="3">
-        <v>9</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" thickBot="1">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="B28" s="3">
-        <v>10</v>
+        <v>12.3</v>
       </c>
       <c r="C28" s="3">
-        <v>20</v>
+        <v>10.4</v>
       </c>
       <c r="D28" s="3">
-        <v>20.2</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" thickBot="1">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
       <c r="B29" s="3">
-        <v>10</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C29" s="3">
-        <v>20</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D29" s="3">
-        <v>20.2</v>
+        <v>5.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: final hcp dashboard update 1/1/26
</commit_message>
<xml_diff>
--- a/shared_data/moyen_indices.xlsx
+++ b/shared_data/moyen_indices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504"/>
+    <workbookView xWindow="4416" yWindow="684" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,25 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>moy_nat</t>
   </si>
@@ -55,13 +69,100 @@
   </si>
   <si>
     <t>09</t>
+  </si>
+  <si>
+    <t>signification_fr</t>
+  </si>
+  <si>
+    <t>Pauvreté multidimensionnelle - 2024</t>
+  </si>
+  <si>
+    <t>Pauvreté multidimensionnelle -2014</t>
+  </si>
+  <si>
+    <t>Scolarisation des enfants (privation)</t>
+  </si>
+  <si>
+    <t>Années de scolarisation (privation)</t>
+  </si>
+  <si>
+    <t>Handicap</t>
+  </si>
+  <si>
+    <t>Mortalité des enfants de moins de 5 ans</t>
+  </si>
+  <si>
+    <t>Électricité</t>
+  </si>
+  <si>
+    <t>Eau potable</t>
+  </si>
+  <si>
+    <t>Assainissement</t>
+  </si>
+  <si>
+    <t>Logement</t>
+  </si>
+  <si>
+    <t>Mode de cuisson</t>
+  </si>
+  <si>
+    <t>Camions</t>
+  </si>
+  <si>
+    <t>Conteneurs à déchets</t>
+  </si>
+  <si>
+    <t>Dans la nature</t>
+  </si>
+  <si>
+    <t>Autres</t>
+  </si>
+  <si>
+    <t>Réseau public d'assainissement</t>
+  </si>
+  <si>
+    <t>Fosse septique</t>
+  </si>
+  <si>
+    <t>Autre</t>
+  </si>
+  <si>
+    <t>Taux d'évolution de la population</t>
+  </si>
+  <si>
+    <t>Taux d'urbanisation</t>
+  </si>
+  <si>
+    <t>Taux de handicap</t>
+  </si>
+  <si>
+    <t>Taux d'analphabétisme</t>
+  </si>
+  <si>
+    <t>Taux de scolarisation (6-11 ans)</t>
+  </si>
+  <si>
+    <t>Préscolaire</t>
+  </si>
+  <si>
+    <t>Primaire</t>
+  </si>
+  <si>
+    <t>Secondaire</t>
+  </si>
+  <si>
+    <t>Lycée</t>
+  </si>
+  <si>
+    <t>Education Supérieure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,13 +176,91 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -148,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -161,6 +340,44 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -169,7 +386,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Mohamed EL AARIFI" id="{A4482CCA-E757-4F97-8B39-352CA72C2022}" userId="S::M.elaarifi@PROVINCEDRIOUCH.onmicrosoft.com::05738b14-0899-49d3-b277-d971a055c9a0" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -455,422 +686,539 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B5" dT="2025-12-30T20:32:05.13" personId="{A4482CCA-E757-4F97-8B39-352CA72C2022}" id="{A037B778-139A-44C1-A8FA-3DBB35080192}">
+    <text>Nombre d’années de scolarité (en situation de privation)</text>
+  </threadedComment>
+  <threadedComment ref="B7" dT="2025-12-30T20:14:12.51" personId="{A4482CCA-E757-4F97-8B39-352CA72C2022}" id="{34F30245-B2AF-4480-8311-30ED08A9CDD4}">
+    <text>Mortalité infantile (en situation de privation)</text>
+  </threadedComment>
+  <threadedComment ref="B13" dT="2025-12-30T20:44:13.93" personId="{A4482CCA-E757-4F97-8B39-352CA72C2022}" id="{AC84D5CB-3BFA-44CF-A897-DD5C47FFFD1E}">
+    <text>Camion de la commune ou privé</text>
+  </threadedComment>
+  <threadedComment ref="B14" dT="2025-12-30T20:35:21.93" personId="{A4482CCA-E757-4F97-8B39-352CA72C2022}" id="{EE71C893-A523-4327-A177-1171CBE5BAA1}">
+    <text>Bac à ordures de la commune</text>
+  </threadedComment>
+  <threadedComment ref="B24" dT="2025-12-30T20:36:57.61" personId="{A4482CCA-E757-4F97-8B39-352CA72C2022}" id="{9FB969DF-7172-4197-BB3D-A28DF2115966}">
+    <text>Taux de scolarisation des 6-11 ans en 2023/2024</text>
+  </threadedComment>
+  <threadedComment ref="B27" dT="2025-12-30T20:20:14.67" personId="{A4482CCA-E757-4F97-8B39-352CA72C2022}" id="{D859D74B-6386-4E22-A2C5-98C48DA8DD69}">
+    <text>Secondaire collégial</text>
+  </threadedComment>
+  <threadedComment ref="B28" dT="2025-12-30T20:20:32.25" personId="{A4482CCA-E757-4F97-8B39-352CA72C2022}" id="{96C4EE71-5CAD-4679-B5DE-A252BC31E8AF}">
+    <text>Secondaire qualifiant</text>
+  </threadedComment>
+  <threadedComment ref="B29" dT="2025-12-30T20:27:41.11" personId="{A4482CCA-E757-4F97-8B39-352CA72C2022}" id="{EE273F85-1529-4AB8-8E93-B7D08144941B}">
+    <text xml:space="preserve">Enseignement supérieur  </text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="8.77734375" style="4"/>
+    <col min="2" max="2" width="31.109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1">
+    <row r="1" spans="1:5" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1">
+    <row r="2" spans="1:5" ht="15" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="13">
         <v>6.8</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="10">
         <v>8.4</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="11">
         <v>11.2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1">
+    <row r="3" spans="1:5" ht="15" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="10">
         <v>11.9</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="11">
         <v>13.5</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="11">
         <v>19.7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1">
+    <row r="4" spans="1:5" ht="15" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="14">
         <v>4.8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="10">
         <v>5.2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="9">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1">
+    <row r="5" spans="1:5" ht="15" thickBot="1">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="12">
         <v>14.6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="15">
         <v>17.2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="11">
         <v>27.2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1">
+    <row r="6" spans="1:5" ht="15" thickBot="1">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="10">
         <v>17</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="15">
         <v>20.399999999999999</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="11">
         <v>26.7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1">
+    <row r="7" spans="1:5" ht="15" thickBot="1">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9">
         <v>0.1</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="9">
         <v>0.1</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1">
+    <row r="8" spans="1:5" ht="15" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="14">
         <v>2.8</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="12">
         <v>3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1">
+    <row r="9" spans="1:5" ht="15" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="16">
         <v>8.3000000000000007</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="14">
         <v>8.6999999999999993</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="11">
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1">
+    <row r="10" spans="1:5" ht="15" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="10">
         <v>12.1</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="14">
         <v>11.9</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="9">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1">
+    <row r="11" spans="1:5" ht="15" thickBot="1">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="18">
         <v>10.7</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="9">
         <v>7.1</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="19">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1">
+    <row r="12" spans="1:5" ht="15" thickBot="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="16">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="9">
         <v>4.5</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1">
+    <row r="13" spans="1:5" ht="15" thickBot="1">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="9">
         <v>56.5</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="18">
         <v>51.9</v>
       </c>
-      <c r="D13" s="3">
+      <c r="E13" s="15">
         <v>23.4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1">
+    <row r="14" spans="1:5" ht="15" thickBot="1">
       <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="10">
         <v>15</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="15">
         <v>21.2</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="10">
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1">
+    <row r="15" spans="1:5" ht="15" thickBot="1">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="10">
         <v>26.6</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="14">
         <v>25.1</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="11">
         <v>53.6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1">
+    <row r="16" spans="1:5" ht="15" thickBot="1">
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="3">
         <v>1.9</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="3">
         <v>1.8</v>
       </c>
-      <c r="D16" s="3">
+      <c r="E16" s="3">
         <v>5.4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1">
+    <row r="17" spans="1:5" ht="15" thickBot="1">
       <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="9">
         <v>65.400000000000006</v>
       </c>
-      <c r="C17" s="3">
+      <c r="D17" s="9">
         <v>65.7</v>
       </c>
-      <c r="D17" s="3">
+      <c r="E17" s="11">
         <v>20.2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1">
+    <row r="18" spans="1:5" ht="15" thickBot="1">
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="9">
         <v>17</v>
       </c>
-      <c r="C18" s="3">
+      <c r="D18" s="16">
         <v>16.2</v>
       </c>
-      <c r="D18" s="3">
+      <c r="E18" s="18">
         <v>15.3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1">
+    <row r="19" spans="1:5" ht="15" thickBot="1">
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="12">
         <v>17.600000000000001</v>
       </c>
-      <c r="C19" s="3">
+      <c r="D19" s="10">
         <v>18.100000000000001</v>
       </c>
-      <c r="D19" s="3">
+      <c r="E19" s="11">
         <v>64.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1">
+    <row r="20" spans="1:5" ht="15" thickBot="1">
       <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="9">
         <v>0.85</v>
       </c>
-      <c r="C20" s="3">
-        <v>0.09</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1">
+      <c r="D20" s="10">
+        <v>-0.09</v>
+      </c>
+      <c r="E20" s="11">
+        <v>-1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1">
       <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="9">
         <v>62.8</v>
       </c>
-      <c r="C21" s="3">
+      <c r="D21" s="9">
         <v>65.599999999999994</v>
       </c>
-      <c r="D21" s="3">
+      <c r="E21" s="15">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1">
+    <row r="22" spans="1:5" ht="15" thickBot="1">
       <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="13">
         <v>4.8</v>
       </c>
-      <c r="C22" s="3">
+      <c r="D22" s="10">
         <v>5.9</v>
       </c>
-      <c r="D22" s="3">
+      <c r="E22" s="11">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1">
+    <row r="23" spans="1:5" ht="15" thickBot="1">
       <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="12">
         <v>24.8</v>
       </c>
-      <c r="C23" s="3">
+      <c r="D23" s="10">
         <v>28.3</v>
       </c>
-      <c r="D23" s="3">
+      <c r="E23" s="11">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1">
+    <row r="24" spans="1:5" ht="15" thickBot="1">
       <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="9">
         <v>95.8</v>
       </c>
-      <c r="C24" s="3">
+      <c r="D24" s="16">
         <v>95</v>
       </c>
-      <c r="D24" s="3">
+      <c r="E24" s="19">
         <v>95.9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1">
+    <row r="25" spans="1:5" ht="15" thickBot="1">
       <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="16">
         <v>1.7</v>
       </c>
-      <c r="C25" s="3">
+      <c r="D25" s="16">
         <v>1.7</v>
       </c>
-      <c r="D25" s="3">
+      <c r="E25" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1">
+    <row r="26" spans="1:5" ht="15" thickBot="1">
       <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="16">
         <v>26.8</v>
       </c>
-      <c r="C26" s="3">
+      <c r="D26" s="18">
         <v>28.8</v>
       </c>
-      <c r="D26" s="3">
+      <c r="E26" s="17">
         <v>30.6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1">
+    <row r="27" spans="1:5" ht="15" thickBot="1">
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="9">
         <v>17.100000000000001</v>
       </c>
-      <c r="C27" s="3">
+      <c r="D27" s="9">
         <v>16.8</v>
       </c>
-      <c r="D27" s="3">
+      <c r="E27" s="14">
         <v>12.7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1">
+    <row r="28" spans="1:5" ht="15" thickBot="1">
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="16">
         <v>12.3</v>
       </c>
-      <c r="C28" s="3">
+      <c r="D28" s="14">
         <v>10.4</v>
       </c>
-      <c r="D28" s="3">
+      <c r="E28" s="11">
         <v>5.2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1">
+    <row r="29" spans="1:5" ht="15" thickBot="1">
       <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="16">
         <v>10.199999999999999</v>
       </c>
-      <c r="C29" s="3">
+      <c r="D29" s="14">
         <v>8.8000000000000007</v>
       </c>
-      <c r="D29" s="3">
+      <c r="E29" s="15">
         <v>5.8</v>
       </c>
     </row>
@@ -886,7 +1234,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -898,7 +1246,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update: final hcp dashboard update 4/1/26
</commit_message>
<xml_diff>
--- a/shared_data/moyen_indices.xlsx
+++ b/shared_data/moyen_indices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4416" yWindow="684" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="57">
   <si>
     <t>moy_nat</t>
   </si>
@@ -155,7 +155,52 @@
     <t>Lycée</t>
   </si>
   <si>
-    <t>Education Supérieure</t>
+    <t>Education Supérieur</t>
+  </si>
+  <si>
+    <t>#FDE9D9</t>
+  </si>
+  <si>
+    <t>#FABF8F</t>
+  </si>
+  <si>
+    <t>#FF0000</t>
+  </si>
+  <si>
+    <t>#FFFF00</t>
+  </si>
+  <si>
+    <t>#92D050</t>
+  </si>
+  <si>
+    <t>#FCD5B4</t>
+  </si>
+  <si>
+    <t>#FFC000</t>
+  </si>
+  <si>
+    <t>#C4D79B</t>
+  </si>
+  <si>
+    <t>#D8E4BC</t>
+  </si>
+  <si>
+    <t>#00B050</t>
+  </si>
+  <si>
+    <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>#EBF1DE</t>
+  </si>
+  <si>
+    <t>c_moy_nat</t>
+  </si>
+  <si>
+    <t>c_moy_reg</t>
+  </si>
+  <si>
+    <t>c_moy_pro</t>
   </si>
 </sst>
 </file>
@@ -327,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -378,6 +423,33 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -386,6 +458,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF92D050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -717,19 +794,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="4"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
     <col min="2" max="2" width="31.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1">
+    <row r="1" spans="1:8" ht="28.2" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -745,8 +825,17 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1">
+      <c r="F1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -762,8 +851,17 @@
       <c r="E2" s="11">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1">
+      <c r="F2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -779,8 +877,17 @@
       <c r="E3" s="11">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1">
+      <c r="F3" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -796,8 +903,17 @@
       <c r="E4" s="9">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1">
+      <c r="F4" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -813,8 +929,17 @@
       <c r="E5" s="11">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1">
+      <c r="F5" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -830,8 +955,17 @@
       <c r="E6" s="11">
         <v>26.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1">
+      <c r="F6" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -847,8 +981,17 @@
       <c r="E7" s="9">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1">
+      <c r="F7" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -864,8 +1007,17 @@
       <c r="E8" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1">
+      <c r="F8" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -881,8 +1033,17 @@
       <c r="E9" s="11">
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1">
+      <c r="F9" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -898,8 +1059,17 @@
       <c r="E10" s="9">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1">
+      <c r="F10" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -915,8 +1085,17 @@
       <c r="E11" s="19">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1">
+      <c r="F11" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -932,8 +1111,17 @@
       <c r="E12" s="19">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1">
+      <c r="F12" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -949,8 +1137,17 @@
       <c r="E13" s="15">
         <v>23.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1">
+      <c r="F13" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -966,8 +1163,17 @@
       <c r="E14" s="10">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1">
+      <c r="F14" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -983,8 +1189,17 @@
       <c r="E15" s="11">
         <v>53.6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1">
+      <c r="F15" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1000,8 +1215,17 @@
       <c r="E16" s="3">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1">
+      <c r="F16" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1017,8 +1241,17 @@
       <c r="E17" s="11">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1">
+      <c r="F17" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1034,8 +1267,17 @@
       <c r="E18" s="18">
         <v>15.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1">
+      <c r="F18" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1051,8 +1293,17 @@
       <c r="E19" s="11">
         <v>64.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1">
+      <c r="F19" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1068,8 +1319,17 @@
       <c r="E20" s="11">
         <v>-1.1399999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1">
+      <c r="F20" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1085,8 +1345,17 @@
       <c r="E21" s="15">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1">
+      <c r="F21" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" thickBot="1">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1102,8 +1371,17 @@
       <c r="E22" s="11">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1">
+      <c r="F22" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" thickBot="1">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1119,8 +1397,17 @@
       <c r="E23" s="11">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1">
+      <c r="F23" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" thickBot="1">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1136,8 +1423,17 @@
       <c r="E24" s="19">
         <v>95.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1">
+      <c r="F24" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1153,8 +1449,17 @@
       <c r="E25" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1">
+      <c r="F25" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1170,8 +1475,17 @@
       <c r="E26" s="17">
         <v>30.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1">
+      <c r="F26" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1187,8 +1501,17 @@
       <c r="E27" s="14">
         <v>12.7</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1">
+      <c r="F27" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" thickBot="1">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1204,8 +1527,17 @@
       <c r="E28" s="11">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1">
+      <c r="F28" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1220,6 +1552,15 @@
       </c>
       <c r="E29" s="15">
         <v>5.8</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1575,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1246,7 +1587,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>